<commit_message>
Remise en forme du code
-Nettoyage du code
-Creation du code en 'XXXX'
-utilisation de char au lieu d'int
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4802" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8733" uniqueCount="244">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -737,6 +737,318 @@
   </si>
   <si>
     <t xml:space="preserve">0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C4
+Code 2 : 5C68B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code 1 : A14C
+Code 2 : 5C68
+Code 3 : 4489
+Code 4 : 8796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789XABCDEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
   </si>
 </sst>
 </file>
@@ -2031,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>183</v>
+        <v>237</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -2299,7 +2611,159 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11"/>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>